<commit_message>
updated Forage Box forms CE1, CE2, On-farm
To include areas to upload photos of the Bare areas, and improve language about walking patterns. Added helper images and helper text. CE2 - v2, CE1 - v1, and On-farm v5
</commit_message>
<xml_diff>
--- a/forms/psa_forage/psa_forage_ce1.xlsx
+++ b/forms/psa_forage/psa_forage_ce1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="29205" yWindow="-1635" windowWidth="37800" windowHeight="19440"/>
+    <workbookView xWindow="29210" yWindow="-1640" windowWidth="37800" windowHeight="19440"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="187">
   <si>
     <t>type</t>
   </si>
@@ -80,9 +80,6 @@
     <t>v1</t>
   </si>
   <si>
-    <t>welcome</t>
-  </si>
-  <si>
     <t>Forage Box Form - for uploading CE1 map files</t>
   </si>
   <si>
@@ -110,9 +107,6 @@
     <t>select_one 1234567</t>
   </si>
   <si>
-    <t>time</t>
-  </si>
-  <si>
     <t>Are you harvesting cover crop biomass at this time?</t>
   </si>
   <si>
@@ -137,15 +131,9 @@
     <t>issues</t>
   </si>
   <si>
-    <t>Do you have any issues to report? (including height of pole and movement of box)</t>
-  </si>
-  <si>
     <t>notes</t>
   </si>
   <si>
-    <t>Take birds eye photos of the cover crops standing inside the cover crops. Hold the tablet chest high, point down, be sure to remove your feet from the image</t>
-  </si>
-  <si>
     <t>image</t>
   </si>
   <si>
@@ -537,13 +525,70 @@
   </si>
   <si>
     <t>Select the fourth treatment you walked in Rep 4</t>
+  </si>
+  <si>
+    <t>rep1_bare</t>
+  </si>
+  <si>
+    <t>begin_group</t>
+  </si>
+  <si>
+    <t>exampleimage1</t>
+  </si>
+  <si>
+    <t>end_group</t>
+  </si>
+  <si>
+    <t>exampleimage2</t>
+  </si>
+  <si>
+    <t>forage_ce1_2.png</t>
+  </si>
+  <si>
+    <t>Image 2: zoom of the walking pattern. Star = flipped up box for 5 seconds while remaining stationary. Then turn the box back to scanning position at height, continuing walking the alley. At the end of the alley (second star) flip the box up again for 5 seconds while remaining stationary. Continue walking to the edge of the plot. Maintaining constant height between tipping is critical. </t>
+  </si>
+  <si>
+    <t>Image1. Example of walking patterns for Forage Box in CE1. Dotted lines represent walking direction across reps. Stars represent start and stop of alleys, where the forage box would be “tipped” for plot/ alley differentiation. Maintaining constant height between tipping is critical. </t>
+  </si>
+  <si>
+    <t>timing</t>
+  </si>
+  <si>
+    <t>rep4_bare</t>
+  </si>
+  <si>
+    <t>rep2_bare</t>
+  </si>
+  <si>
+    <t>Rep 1 Bare</t>
+  </si>
+  <si>
+    <t>Rep 2 Bare</t>
+  </si>
+  <si>
+    <t>Rep 4 Bare</t>
+  </si>
+  <si>
+    <t>Rep 3 Bare</t>
+  </si>
+  <si>
+    <t>notesbarephoto</t>
+  </si>
+  <si>
+    <t>In the following screens, when prompted: Take birds eye photos of the cover crops standing inside the cover crops. Hold the tablet chest high, point down, be sure to remove your feet from the image</t>
+  </si>
+  <si>
+    <t>In the following screens, when prompted: Take birds eye photos of a representative area in the BARE plots.  Hold the tablet chest high, point down, be sure to remove your feet from the image</t>
+  </si>
+  <si>
+    <t>Do you have any comments or issues to report? (including height of pole, movement of box, or plot stand)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -557,13 +602,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -578,9 +635,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -885,23 +950,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H47"/>
+  <dimension ref="A1:H57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="120.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="120.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -927,7 +992,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -935,7 +1000,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -943,7 +1008,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -951,7 +1016,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -959,7 +1024,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -970,13 +1035,13 @@
         <v>14</v>
       </c>
       <c r="E6" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="F6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -993,524 +1058,683 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>169</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>12</v>
       </c>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="B9" t="s">
+        <v>170</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="F9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" t="s">
         <v>20</v>
       </c>
-      <c r="F8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G8" t="s">
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>171</v>
+      </c>
+      <c r="C10" s="3"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>169</v>
+      </c>
+      <c r="C11" s="3"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>171</v>
+      </c>
+      <c r="C13" s="3"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B14" t="s">
         <v>22</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C14" t="s">
         <v>23</v>
       </c>
-      <c r="C9" t="s">
+      <c r="F14" t="s">
         <v>24</v>
       </c>
-      <c r="F9" t="s">
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" t="s">
         <v>26</v>
       </c>
-      <c r="B10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="F15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>27</v>
       </c>
-      <c r="F10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="B16" t="s">
+        <v>176</v>
+      </c>
+      <c r="C16" t="s">
         <v>28</v>
       </c>
-      <c r="B11" t="s">
+      <c r="F16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>104</v>
+      </c>
+      <c r="B17" t="s">
         <v>29</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C17" t="s">
         <v>30</v>
       </c>
-      <c r="F11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>108</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="F17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
         <v>31</v>
       </c>
-      <c r="C12" t="s">
+      <c r="B18" t="s">
         <v>32</v>
       </c>
-      <c r="F12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="C18" t="s">
         <v>33</v>
       </c>
-      <c r="B13" t="s">
+      <c r="F18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>34</v>
       </c>
-      <c r="C13" t="s">
+      <c r="B19" t="s">
+        <v>102</v>
+      </c>
+      <c r="C19" t="s">
+        <v>148</v>
+      </c>
+      <c r="F19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>103</v>
+      </c>
+      <c r="B20" t="s">
+        <v>112</v>
+      </c>
+      <c r="C20" t="s">
+        <v>149</v>
+      </c>
+      <c r="F20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>103</v>
+      </c>
+      <c r="B21" t="s">
+        <v>113</v>
+      </c>
+      <c r="C21" t="s">
+        <v>150</v>
+      </c>
+      <c r="F21" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>103</v>
+      </c>
+      <c r="B22" t="s">
+        <v>114</v>
+      </c>
+      <c r="C22" t="s">
+        <v>151</v>
+      </c>
+      <c r="F22" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>103</v>
+      </c>
+      <c r="B23" t="s">
+        <v>115</v>
+      </c>
+      <c r="C23" t="s">
+        <v>152</v>
+      </c>
+      <c r="F23" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" t="s">
+        <v>109</v>
+      </c>
+      <c r="C24" t="s">
+        <v>153</v>
+      </c>
+      <c r="F24" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>103</v>
+      </c>
+      <c r="B25" t="s">
+        <v>116</v>
+      </c>
+      <c r="C25" t="s">
+        <v>154</v>
+      </c>
+      <c r="F25" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>103</v>
+      </c>
+      <c r="B26" t="s">
+        <v>117</v>
+      </c>
+      <c r="C26" t="s">
+        <v>155</v>
+      </c>
+      <c r="F26" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>103</v>
+      </c>
+      <c r="B27" t="s">
+        <v>118</v>
+      </c>
+      <c r="C27" t="s">
+        <v>156</v>
+      </c>
+      <c r="F27" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>103</v>
+      </c>
+      <c r="B28" t="s">
+        <v>119</v>
+      </c>
+      <c r="C28" t="s">
+        <v>157</v>
+      </c>
+      <c r="F28" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29" t="s">
+        <v>110</v>
+      </c>
+      <c r="C29" t="s">
+        <v>158</v>
+      </c>
+      <c r="F29" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>103</v>
+      </c>
+      <c r="B30" t="s">
+        <v>120</v>
+      </c>
+      <c r="C30" t="s">
+        <v>159</v>
+      </c>
+      <c r="F30" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>103</v>
+      </c>
+      <c r="B31" t="s">
+        <v>121</v>
+      </c>
+      <c r="C31" t="s">
+        <v>160</v>
+      </c>
+      <c r="F31" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>103</v>
+      </c>
+      <c r="B32" t="s">
+        <v>122</v>
+      </c>
+      <c r="C32" t="s">
+        <v>161</v>
+      </c>
+      <c r="F32" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>103</v>
+      </c>
+      <c r="B33" t="s">
+        <v>123</v>
+      </c>
+      <c r="C33" t="s">
+        <v>162</v>
+      </c>
+      <c r="F33" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34" t="s">
+        <v>111</v>
+      </c>
+      <c r="C34" t="s">
+        <v>163</v>
+      </c>
+      <c r="F34" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>103</v>
+      </c>
+      <c r="B35" t="s">
+        <v>124</v>
+      </c>
+      <c r="C35" t="s">
+        <v>164</v>
+      </c>
+      <c r="F35" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>103</v>
+      </c>
+      <c r="B36" t="s">
+        <v>125</v>
+      </c>
+      <c r="C36" t="s">
+        <v>165</v>
+      </c>
+      <c r="F36" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>103</v>
+      </c>
+      <c r="B37" t="s">
+        <v>126</v>
+      </c>
+      <c r="C37" t="s">
+        <v>166</v>
+      </c>
+      <c r="F37" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>103</v>
+      </c>
+      <c r="B38" t="s">
+        <v>127</v>
+      </c>
+      <c r="C38" t="s">
+        <v>167</v>
+      </c>
+      <c r="F38" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>21</v>
+      </c>
+      <c r="B39" t="s">
         <v>35</v>
       </c>
-      <c r="F13" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="C39" t="s">
+        <v>186</v>
+      </c>
+      <c r="F39" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>12</v>
+      </c>
+      <c r="B40" t="s">
         <v>36</v>
       </c>
-      <c r="B14" t="s">
-        <v>106</v>
-      </c>
-      <c r="C14" t="s">
-        <v>152</v>
-      </c>
-      <c r="F14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>107</v>
-      </c>
-      <c r="B15" t="s">
-        <v>116</v>
-      </c>
-      <c r="C15" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>107</v>
-      </c>
-      <c r="B16" t="s">
-        <v>117</v>
-      </c>
-      <c r="C16" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>107</v>
-      </c>
-      <c r="B17" t="s">
-        <v>118</v>
-      </c>
-      <c r="C17" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>107</v>
-      </c>
-      <c r="B18" t="s">
-        <v>119</v>
-      </c>
-      <c r="C18" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" t="s">
-        <v>113</v>
-      </c>
-      <c r="C19" t="s">
-        <v>157</v>
-      </c>
-      <c r="F19" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>107</v>
-      </c>
-      <c r="B20" t="s">
-        <v>120</v>
-      </c>
-      <c r="C20" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>107</v>
-      </c>
-      <c r="B21" t="s">
-        <v>121</v>
-      </c>
-      <c r="C21" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>107</v>
-      </c>
-      <c r="B22" t="s">
-        <v>122</v>
-      </c>
-      <c r="C22" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>107</v>
-      </c>
-      <c r="B23" t="s">
-        <v>123</v>
-      </c>
-      <c r="C23" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>36</v>
-      </c>
-      <c r="B24" t="s">
-        <v>114</v>
-      </c>
-      <c r="C24" t="s">
-        <v>162</v>
-      </c>
-      <c r="F24" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>107</v>
-      </c>
-      <c r="B25" t="s">
-        <v>124</v>
-      </c>
-      <c r="C25" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>107</v>
-      </c>
-      <c r="B26" t="s">
-        <v>125</v>
-      </c>
-      <c r="C26" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>107</v>
-      </c>
-      <c r="B27" t="s">
-        <v>126</v>
-      </c>
-      <c r="C27" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>107</v>
-      </c>
-      <c r="B28" t="s">
-        <v>127</v>
-      </c>
-      <c r="C28" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>36</v>
-      </c>
-      <c r="B29" t="s">
-        <v>115</v>
-      </c>
-      <c r="C29" t="s">
-        <v>167</v>
-      </c>
-      <c r="F29" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>107</v>
-      </c>
-      <c r="B30" t="s">
-        <v>128</v>
-      </c>
-      <c r="C30" t="s">
+      <c r="C40" t="s">
+        <v>184</v>
+      </c>
+      <c r="F40" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>12</v>
+      </c>
+      <c r="B41" t="s">
+        <v>183</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="F41" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>37</v>
+      </c>
+      <c r="B42" t="s">
+        <v>38</v>
+      </c>
+      <c r="C42" t="s">
+        <v>39</v>
+      </c>
+      <c r="F42" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>37</v>
+      </c>
+      <c r="B43" t="s">
+        <v>40</v>
+      </c>
+      <c r="C43" t="s">
+        <v>41</v>
+      </c>
+      <c r="F43" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>37</v>
+      </c>
+      <c r="B44" t="s">
+        <v>42</v>
+      </c>
+      <c r="C44" t="s">
+        <v>43</v>
+      </c>
+      <c r="F44" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>37</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>107</v>
-      </c>
-      <c r="B31" t="s">
-        <v>129</v>
-      </c>
-      <c r="C31" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>107</v>
-      </c>
-      <c r="B32" t="s">
-        <v>130</v>
-      </c>
-      <c r="C32" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>107</v>
-      </c>
-      <c r="B33" t="s">
-        <v>131</v>
-      </c>
-      <c r="C33" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>22</v>
-      </c>
-      <c r="B34" t="s">
+      <c r="C45" t="s">
+        <v>179</v>
+      </c>
+      <c r="F45" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
         <v>37</v>
       </c>
-      <c r="C34" t="s">
-        <v>38</v>
-      </c>
-      <c r="F34" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>12</v>
-      </c>
-      <c r="B35" t="s">
-        <v>39</v>
-      </c>
-      <c r="C35" t="s">
-        <v>40</v>
-      </c>
-      <c r="F35" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>41</v>
-      </c>
-      <c r="B36" t="s">
-        <v>42</v>
-      </c>
-      <c r="C36" t="s">
-        <v>43</v>
-      </c>
-      <c r="F36" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>41</v>
-      </c>
-      <c r="B37" t="s">
+      <c r="B46" t="s">
         <v>44</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C46" t="s">
         <v>45</v>
       </c>
-      <c r="F37" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>41</v>
-      </c>
-      <c r="B38" t="s">
+      <c r="F46" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>37</v>
+      </c>
+      <c r="B47" t="s">
         <v>46</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C47" t="s">
         <v>47</v>
       </c>
-      <c r="F38" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>41</v>
-      </c>
-      <c r="B39" t="s">
+      <c r="F47" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>37</v>
+      </c>
+      <c r="B48" t="s">
         <v>48</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C48" t="s">
         <v>49</v>
       </c>
-      <c r="F39" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>41</v>
-      </c>
-      <c r="B40" t="s">
+      <c r="F48" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>37</v>
+      </c>
+      <c r="B49" t="s">
+        <v>178</v>
+      </c>
+      <c r="C49" t="s">
+        <v>180</v>
+      </c>
+      <c r="F49" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>37</v>
+      </c>
+      <c r="B50" t="s">
         <v>50</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C50" t="s">
         <v>51</v>
       </c>
-      <c r="F40" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>41</v>
-      </c>
-      <c r="B41" t="s">
+      <c r="F50" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>37</v>
+      </c>
+      <c r="B51" t="s">
         <v>52</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C51" t="s">
         <v>53</v>
       </c>
-      <c r="F41" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>41</v>
-      </c>
-      <c r="B42" t="s">
+      <c r="F51" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>37</v>
+      </c>
+      <c r="B52" t="s">
         <v>54</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C52" t="s">
         <v>55</v>
       </c>
-      <c r="F42" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>41</v>
-      </c>
-      <c r="B43" t="s">
+      <c r="F52" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>37</v>
+      </c>
+      <c r="B53" t="s">
+        <v>177</v>
+      </c>
+      <c r="C53" t="s">
+        <v>182</v>
+      </c>
+      <c r="F53" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>37</v>
+      </c>
+      <c r="B54" t="s">
         <v>56</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C54" t="s">
         <v>57</v>
       </c>
-      <c r="F43" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>41</v>
-      </c>
-      <c r="B44" t="s">
+      <c r="F54" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>37</v>
+      </c>
+      <c r="B55" t="s">
         <v>58</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C55" t="s">
         <v>59</v>
       </c>
-      <c r="F44" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>41</v>
-      </c>
-      <c r="B45" t="s">
+      <c r="F55" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>37</v>
+      </c>
+      <c r="B56" t="s">
         <v>60</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C56" t="s">
         <v>61</v>
       </c>
-      <c r="F45" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>41</v>
-      </c>
-      <c r="B46" t="s">
-        <v>62</v>
-      </c>
-      <c r="C46" t="s">
-        <v>63</v>
-      </c>
-      <c r="F46" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>41</v>
-      </c>
-      <c r="B47" t="s">
-        <v>64</v>
-      </c>
-      <c r="C47" t="s">
-        <v>65</v>
-      </c>
-      <c r="F47" t="s">
+      <c r="F56" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>37</v>
+      </c>
+      <c r="B57" t="s">
+        <v>177</v>
+      </c>
+      <c r="C57" t="s">
+        <v>181</v>
+      </c>
+      <c r="F57" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1522,14 +1746,14 @@
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -1538,323 +1762,323 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" t="s">
         <v>67</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>68</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B4" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="C4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" t="s">
         <v>67</v>
       </c>
-      <c r="B3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B4" t="s">
-        <v>73</v>
-      </c>
-      <c r="C4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>72</v>
-      </c>
-      <c r="B6" t="s">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>77</v>
       </c>
-      <c r="C6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>72</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="B9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>79</v>
       </c>
-      <c r="C7" t="s">
+      <c r="B10" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="C10" t="s">
         <v>81</v>
       </c>
-      <c r="B8" t="s">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>79</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
         <v>82</v>
       </c>
-      <c r="C8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>81</v>
-      </c>
-      <c r="B9" t="s">
-        <v>68</v>
-      </c>
-      <c r="C9" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>83</v>
-      </c>
-      <c r="B10" t="s">
-        <v>84</v>
-      </c>
-      <c r="C10" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>83</v>
-      </c>
-      <c r="B11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>98765</v>
       </c>
       <c r="B12" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C12" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>98765</v>
       </c>
       <c r="B13" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C13" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>98765</v>
       </c>
       <c r="B14" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C14" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>98765</v>
       </c>
       <c r="B15" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C15" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>98765</v>
       </c>
       <c r="B16" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C16" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>98765</v>
       </c>
       <c r="B17" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C17" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>98765</v>
       </c>
       <c r="B18" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C18" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>98765</v>
       </c>
       <c r="B19" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C19" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>98765</v>
       </c>
       <c r="B20" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C20" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>98765</v>
       </c>
       <c r="B21" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C21" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>98765</v>
       </c>
       <c r="B22" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C22" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>98765</v>
       </c>
       <c r="B23" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C23" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>98765</v>
       </c>
       <c r="B24" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C24" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>98765</v>
       </c>
       <c r="B25" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C25" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>98765</v>
       </c>
       <c r="B26" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C26" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>987</v>
       </c>
       <c r="B27" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C27" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>987</v>
       </c>
       <c r="B28" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C28" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>987</v>
       </c>
       <c r="B29" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C29" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>987</v>
       </c>
       <c r="B30" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C30" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -1868,22 +2092,22 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>